<commit_message>
Added new Test data file
Added new Test data file
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>Chart1</t>
-  </si>
-  <si>
-    <t>Chart2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Chart3</t>
   </si>
@@ -37,6 +31,36 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>Test Case#</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>Trust RR8 vs Region R1</t>
+  </si>
+  <si>
+    <t>Trust RR8 vs Peers</t>
+  </si>
+  <si>
+    <t>Trust RR1 vs Peers</t>
   </si>
 </sst>
 </file>
@@ -370,82 +394,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>

</xml_diff>

<commit_message>
Scripts updated for application changes
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Chart3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>UserName</t>
   </si>
@@ -30,37 +27,43 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>Test Case#</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>Trust_Name</t>
+  </si>
+  <si>
+    <t>RR8</t>
+  </si>
+  <si>
+    <t>Initial Label</t>
+  </si>
+  <si>
+    <t>Expected Graph Label</t>
+  </si>
+  <si>
+    <t>Region R1 and Others</t>
+  </si>
+  <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>others</t>
-  </si>
-  <si>
-    <t>Test Case#</t>
-  </si>
-  <si>
-    <t>TC01</t>
-  </si>
-  <si>
-    <t>TC02</t>
-  </si>
-  <si>
-    <t>TC03</t>
-  </si>
-  <si>
-    <t>TC04</t>
-  </si>
-  <si>
-    <t>Trust RR8 vs Region R1</t>
-  </si>
-  <si>
-    <t>Trust RR8 vs Peers</t>
-  </si>
-  <si>
-    <t>Trust RR1 vs Peers</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,13 +110,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,75 +412,93 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added automation test case changes for ubuntu
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Trust_Name</t>
   </si>
   <si>
-    <t>RR8</t>
-  </si>
-  <si>
     <t>Initial Label</t>
   </si>
   <si>
@@ -64,6 +61,12 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>RR1</t>
+  </si>
+  <si>
+    <t>Derived waiting time</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,13 +432,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -454,10 +457,10 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -468,10 +471,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,13 +482,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -493,13 +496,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added API Validation for Trust values
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>UserName</t>
   </si>
@@ -57,23 +57,38 @@
     <t>Expected Graph Label</t>
   </si>
   <si>
-    <t>Region R1 and Others</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>RR1</t>
-  </si>
-  <si>
-    <t>Derived waiting time</t>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>Derived waiting time of underlying region R1 with other regions R3,R2,R4</t>
+  </si>
+  <si>
+    <t>AUT</t>
+  </si>
+  <si>
+    <t>Derived waiting time of trust AUT with its underlying region R1</t>
+  </si>
+  <si>
+    <t>Derived waiting time of trust AUT with peers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +96,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -114,24 +143,171 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,125 +588,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1">
+        <v>57.340909090909001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>56.590909090909001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>61.079545454545404</v>
+      </c>
+      <c r="H3" s="6">
+        <v>72.920454545454504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>57.340909090909001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>56.590909090909001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>61.079545454545404</v>
+      </c>
+      <c r="H4" s="6">
+        <v>72.920454545454504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Home Page Code updated
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -72,9 +72,6 @@
     <t>E4</t>
   </si>
   <si>
-    <t>Derived waiting time of underlying region R1 with other regions R3,R2,R4</t>
-  </si>
-  <si>
     <t>AUT</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Derived waiting time of trust AUT with peers</t>
+  </si>
+  <si>
+    <t>Derived waiting time of trust AUT</t>
   </si>
 </sst>
 </file>
@@ -588,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,10 +665,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1">
@@ -689,13 +689,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>57.340909090909001</v>
@@ -710,18 +710,18 @@
         <v>72.920454545454504</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -778,6 +778,9 @@
       <c r="G10" s="8"/>
       <c r="H10" s="10"/>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ubuntu related changes done
</commit_message>
<xml_diff>
--- a/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
+++ b/NHS.Automation/FrameworkPython/test_data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>UserName</t>
   </si>
@@ -81,7 +81,13 @@
     <t>Derived waiting time of trust AUT with peers</t>
   </si>
   <si>
-    <t>Derived waiting time of trust AUT</t>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Derived waiting time of underlying region R1</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -273,11 +279,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,6 +329,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G7" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +629,7 @@
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
@@ -629,17 +654,20 @@
       <c r="H1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -656,11 +684,14 @@
       <c r="J2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -684,7 +715,7 @@
         <v>72.920454545454504</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -710,7 +741,7 @@
         <v>72.920454545454504</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -721,14 +752,14 @@
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -738,7 +769,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -748,7 +779,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -758,7 +789,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -768,7 +799,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -778,7 +809,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
     </row>
   </sheetData>

</xml_diff>